<commit_message>
add mid query to net task handler
</commit_message>
<xml_diff>
--- a/docs/端口映射申请表CENI-1215-1729.xlsx
+++ b/docs/端口映射申请表CENI-1215-1729.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
   <si>
     <t>目录</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>192.168.143.5</t>
+  </si>
+  <si>
+    <t>WebSocket</t>
+  </si>
+  <si>
+    <t>Sun FrontEnd</t>
+  </si>
+  <si>
+    <t>Log Server</t>
+  </si>
+  <si>
+    <t>ZMQ</t>
   </si>
 </sst>
 </file>
@@ -1235,16 +1247,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>960755</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6985</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>74930</xdr:rowOff>
+      <xdr:rowOff>27305</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>508635</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>1088390</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1261,8 +1273,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1671955" y="3229610"/>
-          <a:ext cx="4098925" cy="3359785"/>
+          <a:off x="2021840" y="3181985"/>
+          <a:ext cx="4328795" cy="3542030"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1722,12 +1734,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -2119,6 +2131,26 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
+    <row r="18" spans="7:7">
+      <c r="G18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7">
+      <c r="G19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7">
+      <c r="G20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7">
+      <c r="G21" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:K13"/>
   <mergeCells count="1">

</xml_diff>